<commit_message>
cambio de logica para subir registros, asi hallan repetidos va a subor el que sea nuevo
</commit_message>
<xml_diff>
--- a/public/datos_volcar.xlsx
+++ b/public/datos_volcar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathan\Desktop\talent\telentoTechLocal\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76648268-2014-4930-B658-834C0AD40BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2F6730-7B74-4A0B-8556-368CED5AD9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36FD603F-CBB0-4648-8E3B-6C95393CCE26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="166">
   <si>
     <t>id</t>
   </si>
@@ -528,13 +528,19 @@
   </si>
   <si>
     <t>password40</t>
+  </si>
+  <si>
+    <t>password41</t>
+  </si>
+  <si>
+    <t>chloerogers1@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +558,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -574,14 +588,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -914,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C678D3E-7D42-48AB-86C5-B522468E642C}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,9 +1641,32 @@
         <v>163</v>
       </c>
     </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E44" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D42" r:id="rId1" xr:uid="{83889DBB-62BC-4810-A025-E0EB5248F94E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>